<commit_message>
Client asked to change that line. Closes-bug:12
</commit_message>
<xml_diff>
--- a/bill-final.xlsx
+++ b/bill-final.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spanc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spanc\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Swathi Spent</t>
   </si>
@@ -443,7 +443,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,6 +533,13 @@
         <f>B2</f>
         <v>5.48</v>
       </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <f>E6/2</f>
+        <v>6.8125</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">

</xml_diff>